<commit_message>
minor changes and xsdir bug correction
xsdir pyne bug correction
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laghi\Documents\03_dottorato\04_F4E\01_JADE\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D42D307-85BD-4F39-A075-5F840EB0B7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DE2CD5-A758-4AB2-8981-C4437EE8D7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -155,7 +155,7 @@
     <t>Activation (NI)</t>
   </si>
   <si>
-    <t>C:\Users\laghi\Documents\MCNP\MCNP_DATA\xsdir</t>
+    <t>C:\Users\laghi\Documents\MCNP\MCNP_DATA\xsdir_mcnp6.2</t>
   </si>
 </sst>
 </file>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A1A2DE-3EB8-4AD4-9CF1-023800AFF144}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
begin pp of comp benchmark
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laghi\Documents\03_dottorato\04_F4E\01_JADE\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E564FA57-9676-4A33-9947-F319DA80A769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B52C15-54DC-4576-913C-174DCAE6F051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="2220" windowWidth="17472" windowHeight="8412" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -787,7 +787,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,10 +869,10 @@
         <v>40</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="12">
         <v>10000</v>
@@ -901,7 +901,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F5" s="12">
         <v>10000</v>

</xml_diff>